<commit_message>
Modifications of ViewEditForm logic
</commit_message>
<xml_diff>
--- a/Programari.xlsx
+++ b/Programari.xlsx
@@ -4,36 +4,37 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="16-JUL-2023" sheetId="22" r:id="rId1"/>
-    <sheet name="10-JUN-2023" sheetId="21" r:id="rId2"/>
-    <sheet name="23-APR-2023" sheetId="20" r:id="rId3"/>
-    <sheet name="20-APR-2023" sheetId="19" r:id="rId4"/>
-    <sheet name="6-APR-2023" sheetId="13" r:id="rId5"/>
-    <sheet name="4-APR-2023" sheetId="17" r:id="rId6"/>
-    <sheet name="3-APR-2023" sheetId="16" r:id="rId7"/>
-    <sheet name="2-APR-2023" sheetId="5" r:id="rId8"/>
-    <sheet name="1-APR-2023" sheetId="14" r:id="rId9"/>
-    <sheet name="31-MAR-2023" sheetId="18" r:id="rId10"/>
-    <sheet name="30-MAR-2023" sheetId="15" r:id="rId11"/>
-    <sheet name="29-MAR-2023" sheetId="12" r:id="rId12"/>
-    <sheet name="28-MAR-2023" sheetId="10" r:id="rId13"/>
-    <sheet name="27-MAR-2023" sheetId="6" r:id="rId14"/>
-    <sheet name="26-MAR-2023" sheetId="11" r:id="rId15"/>
-    <sheet name="25-MAR-2023" sheetId="7" r:id="rId16"/>
-    <sheet name="24-MAR-2023" sheetId="8" r:id="rId17"/>
-    <sheet name="23-MAR-2023" sheetId="4" r:id="rId18"/>
-    <sheet name="Header" sheetId="1" state="hidden" r:id="rId19"/>
-    <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId20"/>
+    <sheet name="7-SEP-2023" sheetId="23" r:id="rId1"/>
+    <sheet name="16-JUL-2023" sheetId="22" r:id="rId2"/>
+    <sheet name="10-JUN-2023" sheetId="21" r:id="rId3"/>
+    <sheet name="23-APR-2023" sheetId="20" r:id="rId4"/>
+    <sheet name="20-APR-2023" sheetId="19" r:id="rId5"/>
+    <sheet name="6-APR-2023" sheetId="13" r:id="rId6"/>
+    <sheet name="4-APR-2023" sheetId="17" r:id="rId7"/>
+    <sheet name="3-APR-2023" sheetId="16" r:id="rId8"/>
+    <sheet name="2-APR-2023" sheetId="5" r:id="rId9"/>
+    <sheet name="1-APR-2023" sheetId="14" r:id="rId10"/>
+    <sheet name="31-MAR-2023" sheetId="18" r:id="rId11"/>
+    <sheet name="30-MAR-2023" sheetId="15" r:id="rId12"/>
+    <sheet name="29-MAR-2023" sheetId="12" r:id="rId13"/>
+    <sheet name="28-MAR-2023" sheetId="10" r:id="rId14"/>
+    <sheet name="27-MAR-2023" sheetId="6" r:id="rId15"/>
+    <sheet name="26-MAR-2023" sheetId="11" r:id="rId16"/>
+    <sheet name="25-MAR-2023" sheetId="7" r:id="rId17"/>
+    <sheet name="24-MAR-2023" sheetId="8" r:id="rId18"/>
+    <sheet name="23-MAR-2023" sheetId="4" r:id="rId19"/>
+    <sheet name="Header" sheetId="1" state="hidden" r:id="rId20"/>
+    <sheet name="Sheet1" sheetId="2" state="hidden" r:id="rId21"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="52">
   <si>
     <t xml:space="preserve"> NUME PACIENT</t>
   </si>
@@ -677,10 +678,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -795,10 +795,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
         <v>45</v>
@@ -838,6 +838,170 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet12"/>
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="60.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5">
+        <f>COUNTA(B2:B20)</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="5">
+        <f>COUNTIF(D2:D20,"DA")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A10:F10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:F20"/>
@@ -1001,7 +1165,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:F20"/>
@@ -1156,7 +1320,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:F20"/>
@@ -1311,7 +1475,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:F20"/>
@@ -1466,7 +1630,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:F20"/>
@@ -1621,7 +1785,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:F20"/>
@@ -1776,7 +1940,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F20"/>
@@ -1958,7 +2122,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:F20"/>
@@ -2113,7 +2277,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F20"/>
@@ -2268,7 +2432,169 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet20"/>
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="60.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5">
+        <f>COUNTA(B2:B20)</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="5">
+        <f>COUNTIF(D2:D20,"DA")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A10:F10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F20"/>
@@ -2423,169 +2749,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet19"/>
-  <dimension ref="A1:F20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="60.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="5">
-        <f>COUNTA(B2:B20)</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="5">
-        <f>COUNTIF(D2:D20,"DA")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A10:F10"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
@@ -2610,6 +2774,168 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet19"/>
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="60.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5">
+        <f>COUNTA(B2:B20)</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="5">
+        <f>COUNTIF(D2:D20,"DA")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A10:F10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -2767,7 +3093,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:F20"/>
@@ -2920,12 +3246,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3082,7 +3408,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:F20"/>
@@ -3243,7 +3569,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:F20"/>
@@ -3413,7 +3739,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F20"/>
@@ -3578,168 +3904,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet12"/>
-  <dimension ref="A1:F20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="35.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="60.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="5">
-        <f>COUNTA(B2:B20)</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="5">
-        <f>COUNTIF(D2:D20,"DA")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A10:F10"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>